<commit_message>
Completed ability to bulk upload gatecodes Needed to make some modifications to the database because the gate code could not be used as a primary key (duplicate values possible) Added verbiage for 72 rule on the login page
</commit_message>
<xml_diff>
--- a/Testing Checklist.xlsx
+++ b/Testing Checklist.xlsx
@@ -5,17 +5,18 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jason\OneDrive\Documents\Practicum\VIPParking\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jason\OneDrive\Documents\Practicum\vip2\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530"/>
   </bookViews>
   <sheets>
     <sheet name="Home Page" sheetId="1" r:id="rId1"/>
     <sheet name="Login" sheetId="2" r:id="rId2"/>
     <sheet name="Reservations" sheetId="3" r:id="rId3"/>
-    <sheet name="Reports" sheetId="4" r:id="rId4"/>
+    <sheet name="Categories" sheetId="5" r:id="rId4"/>
+    <sheet name="Reports" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="158">
   <si>
     <t>Test</t>
   </si>
@@ -447,6 +448,118 @@
   </si>
   <si>
     <t>Admin filters report by category or department</t>
+  </si>
+  <si>
+    <t>Non-admin tries to access Categories page</t>
+  </si>
+  <si>
+    <t>:/Categories</t>
+  </si>
+  <si>
+    <t>Redirected to Not Found page</t>
+  </si>
+  <si>
+    <t>Admin accesses Categories page</t>
+  </si>
+  <si>
+    <t>Sees list of existing categories with CRUD abilities</t>
+  </si>
+  <si>
+    <t>Non-admin tries to access Categories details page</t>
+  </si>
+  <si>
+    <t>:/Categories/Details/&lt;Category ID&gt;</t>
+  </si>
+  <si>
+    <t>Admin tries to access Categories details page without an ID</t>
+  </si>
+  <si>
+    <t>:/Categories/Details/</t>
+  </si>
+  <si>
+    <t>Redirected to Bad Request</t>
+  </si>
+  <si>
+    <t>Admin tries to access Categories details page with an invalid ID</t>
+  </si>
+  <si>
+    <t>:/Categories/Details/&lt;invalid ID&gt;</t>
+  </si>
+  <si>
+    <t>Admin accesses a valid Categories details page</t>
+  </si>
+  <si>
+    <t>Sees details of category</t>
+  </si>
+  <si>
+    <t>Admin tries to create category without a title</t>
+  </si>
+  <si>
+    <t>:/Categories/Create</t>
+  </si>
+  <si>
+    <t>Title = &lt;blank&gt;</t>
+  </si>
+  <si>
+    <t>Form is return with validation errors</t>
+  </si>
+  <si>
+    <t>Admin successfully creates a category</t>
+  </si>
+  <si>
+    <t>Category is added to the database
+Redirected back to Categories Index page with new category on the list</t>
+  </si>
+  <si>
+    <t>Non-admin tries to access Categories edit page</t>
+  </si>
+  <si>
+    <t>Admin tries to access Categories edit page without an ID</t>
+  </si>
+  <si>
+    <t>Admin tries to access Categories edit page with an invalid ID</t>
+  </si>
+  <si>
+    <t>Admin accesses a valid Categories edit page</t>
+  </si>
+  <si>
+    <t>Admin successfully edits a category</t>
+  </si>
+  <si>
+    <t>:/Categories/Edit/</t>
+  </si>
+  <si>
+    <t>:/Categories/Edit/&lt;invalid ID&gt;</t>
+  </si>
+  <si>
+    <t>:/Categories/Edit/&lt;Category ID&gt;</t>
+  </si>
+  <si>
+    <t>Sees a form to edit the title of the category</t>
+  </si>
+  <si>
+    <t>Category is modified in the database
+Redirected back to Categories Index page</t>
+  </si>
+  <si>
+    <t>Non-admin tries to delete a category</t>
+  </si>
+  <si>
+    <t>:/Categories/Delete/&lt;Category ID&gt;</t>
+  </si>
+  <si>
+    <t>Redirect to Not Found page</t>
+  </si>
+  <si>
+    <t>Admin deletes a category</t>
+  </si>
+  <si>
+    <t>Redirected to an "Are you sure" screen
+If confirmed, category is deleted from the database
+Redirect back to Index page</t>
+  </si>
+  <si>
+    <t>p</t>
   </si>
 </sst>
 </file>
@@ -812,13 +925,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="110.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="38.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="38.28515625" customWidth="1"/>
     <col min="3" max="3" width="33.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="62.42578125" bestFit="1" customWidth="1"/>
@@ -851,6 +964,9 @@
       <c r="D3" t="s">
         <v>4</v>
       </c>
+      <c r="E3" t="s">
+        <v>157</v>
+      </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -861,6 +977,9 @@
       </c>
       <c r="D4" t="s">
         <v>9</v>
+      </c>
+      <c r="E4" t="s">
+        <v>157</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -876,7 +995,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
@@ -1146,7 +1265,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>47</v>
       </c>
@@ -1444,9 +1563,215 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="57.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="46" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>122</v>
+      </c>
+      <c r="B2" t="s">
+        <v>123</v>
+      </c>
+      <c r="D2" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>125</v>
+      </c>
+      <c r="B3" t="s">
+        <v>123</v>
+      </c>
+      <c r="D3" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>127</v>
+      </c>
+      <c r="B4" t="s">
+        <v>128</v>
+      </c>
+      <c r="D4" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>129</v>
+      </c>
+      <c r="B5" t="s">
+        <v>130</v>
+      </c>
+      <c r="D5" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>132</v>
+      </c>
+      <c r="B6" t="s">
+        <v>133</v>
+      </c>
+      <c r="D6" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>134</v>
+      </c>
+      <c r="B7" t="s">
+        <v>128</v>
+      </c>
+      <c r="D7" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>136</v>
+      </c>
+      <c r="B8" t="s">
+        <v>137</v>
+      </c>
+      <c r="C8" t="s">
+        <v>138</v>
+      </c>
+      <c r="D8" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>140</v>
+      </c>
+      <c r="B9" t="s">
+        <v>137</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>142</v>
+      </c>
+      <c r="B10" t="s">
+        <v>128</v>
+      </c>
+      <c r="D10" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>143</v>
+      </c>
+      <c r="B11" t="s">
+        <v>147</v>
+      </c>
+      <c r="D11" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>144</v>
+      </c>
+      <c r="B12" t="s">
+        <v>148</v>
+      </c>
+      <c r="D12" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>145</v>
+      </c>
+      <c r="B13" t="s">
+        <v>149</v>
+      </c>
+      <c r="D13" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>146</v>
+      </c>
+      <c r="B14" t="s">
+        <v>149</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>152</v>
+      </c>
+      <c r="B15" t="s">
+        <v>153</v>
+      </c>
+      <c r="D15" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>155</v>
+      </c>
+      <c r="B16" t="s">
+        <v>153</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>156</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>

</xml_diff>